<commit_message>
updated bdesc, baepabcip, bgdpbes, cdrdfrcp, csc, eiae, mcf, bs, fpiebp, mpiifp, fopity, vsbs, beacp
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BAEPAbCiPC/Bool Are Energy Prices Affected by Chng in Production Costs.xlsx
+++ b/InputData/ctrl-settings/BAEPAbCiPC/Bool Are Energy Prices Affected by Chng in Production Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ctrl-settings\BAEPAbCiPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\RMI\RMI_all_states\CO\ctrl-settings\BAEPAbCiPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE9E4214-784F-4D93-88A1-FAA20AFC8BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9224171C-26A0-4E27-A396-DE32F1375B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15450" yWindow="135" windowWidth="13350" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Source:</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Unit: boolean (1 or 0)</t>
+  </si>
+  <si>
+    <t>Colorado</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,20 +478,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="5">
+        <v>45271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,32 +505,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -539,46 +548,46 @@
   </sheetPr>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.81640625" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -586,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -594,7 +603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -602,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -610,63 +619,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -674,39 +683,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -714,11 +723,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22">
         <v>1</v>
       </c>
     </row>

</xml_diff>